<commit_message>
eid ul fitre-23 er por
</commit_message>
<xml_diff>
--- a/DataScience/BasicPython/Drawable/dateSet.xlsx
+++ b/DataScience/BasicPython/Drawable/dateSet.xlsx
@@ -476,16 +476,16 @@
         <v>44072</v>
       </c>
       <c r="B2" t="n">
-        <v>1.327869765796777</v>
+        <v>-1.370798257884184</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.2064063237256248</v>
+        <v>-0.9727079006722509</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.120898237076419</v>
+        <v>0.3038797348144729</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7675060982390984</v>
+        <v>-0.9595538525665909</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -499,16 +499,16 @@
         <v>44073</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.891466893484395</v>
+        <v>-0.08261641856586049</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.2064765562551106</v>
+        <v>-0.3163358775390812</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.5567295215797187</v>
+        <v>-0.1806755391691144</v>
       </c>
       <c r="E3" t="n">
-        <v>0.906382289222716</v>
+        <v>-0.1934911213520627</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -522,16 +522,16 @@
         <v>44074</v>
       </c>
       <c r="B4" t="n">
-        <v>1.143592852646202</v>
+        <v>-0.8290690241082486</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.450352792126658</v>
+        <v>-0.09790517462118323</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.8888220961446109</v>
+        <v>0.435524577543085</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.886422231479767</v>
+        <v>1.013510180591872</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -545,16 +545,16 @@
         <v>44075</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.2053485988567079</v>
+        <v>0.6106966230070665</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2377963168514883</v>
+        <v>-0.4540586176844206</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.8589107392809182</v>
+        <v>-0.5976933272505026</v>
       </c>
       <c r="E5" t="n">
-        <v>1.068946822780671</v>
+        <v>0.8935945057248388</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -568,16 +568,16 @@
         <v>44076</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.01963623469267269</v>
+        <v>1.546965732314469</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.4755537946611942</v>
+        <v>-0.3393215870801091</v>
       </c>
       <c r="D6" t="n">
-        <v>1.463402396004526</v>
+        <v>0.1707791176747497</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0824106742083771</v>
+        <v>-1.304386256282822</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -591,16 +591,16 @@
         <v>44077</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.8428461942137967</v>
+        <v>-0.8093931452109928</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.5389611858134592</v>
+        <v>-1.090172000347444</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.3212230815083802</v>
+        <v>-0.4531575605523151</v>
       </c>
       <c r="E7" t="n">
-        <v>-1.023501221212854</v>
+        <v>-1.792323026094754</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>

</xml_diff>